<commit_message>
modified:   Antispritzschutz_Daten_Liner_4.xlsx 	modified:   Antispritzschutz_Daten_Liner_5.xlsx 	modified:   "Liner 4 Sch\303\274rzen/511128907-0.plt" 	new file:   "Liner 4 Sch\303\274rzen/511128912-0.plt" 	new file:   "Liner 4 Sch\303\274rzen/versuch 2.plt" 	new file:   "Liner 4 Sch\303\274rzen/versuch1.plt"
</commit_message>
<xml_diff>
--- a/Antispritzschutz_Daten_Liner_5.xlsx
+++ b/Antispritzschutz_Daten_Liner_5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Programme\Script Zeichnung erstellen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Programme\Programm_HPGL_Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F520091-33C2-4378-90C7-381EF292A21F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F1FE32-CBC5-43F1-9692-44978FC166FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Modell Nr.</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Länge Schürze</t>
+  </si>
+  <si>
+    <t>Erstellungsdatum</t>
   </si>
 </sst>
 </file>
@@ -85,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,15 +371,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,8 +401,11 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -413,6 +423,9 @@
       </c>
       <c r="F2" t="s">
         <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>36488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>